<commit_message>
need DTAIL and SPEC
</commit_message>
<xml_diff>
--- a/P13/Scrum.xlsx
+++ b/P13/Scrum.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rachaelrocha/Documents/GitHub/cse1325/P11/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rachaelrocha/Documents/GitHub/cse1325/P13/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79741BFC-988F-3D40-9390-E2E3F1DDA0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B963EF4-6E37-7A4E-AE1F-586739160CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30160" windowHeight="17100" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30160" windowHeight="17100" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="171">
   <si>
     <t>Product Name:</t>
   </si>
@@ -549,6 +549,12 @@
   </si>
   <si>
     <t>Completed Day 7</t>
+  </si>
+  <si>
+    <t>Finished in Sprint 6</t>
+  </si>
+  <si>
+    <t>Completed Day 2</t>
   </si>
 </sst>
 </file>
@@ -559,7 +565,7 @@
     <numFmt numFmtId="164" formatCode="mmm\ dd"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -622,6 +628,12 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -709,7 +721,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -825,6 +837,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -840,8 +855,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2932,28 +2947,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3738,8 +3753,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView topLeftCell="A44" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3762,14 +3777,14 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
       <c r="H1" s="5"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
@@ -3780,12 +3795,12 @@
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -3824,66 +3839,66 @@
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="48" t="s">
         <v>161</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
       <c r="H5" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="I5" s="48">
+      <c r="I5" s="43">
         <v>1001828709</v>
       </c>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="5"/>
@@ -4111,10 +4126,10 @@
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
-      <c r="F22" s="44" t="s">
+      <c r="F22" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="44"/>
+      <c r="G22" s="45"/>
       <c r="H22" s="13"/>
       <c r="I22" s="13" t="s">
         <v>19</v>
@@ -4982,7 +4997,9 @@
         <v>5</v>
       </c>
       <c r="F51" s="17"/>
-      <c r="G51" s="17"/>
+      <c r="G51" s="17" t="s">
+        <v>169</v>
+      </c>
       <c r="H51" s="18" t="s">
         <v>119</v>
       </c>
@@ -5009,7 +5026,9 @@
         <v>13</v>
       </c>
       <c r="F52" s="17"/>
-      <c r="G52" s="17"/>
+      <c r="G52" s="17" t="s">
+        <v>169</v>
+      </c>
       <c r="H52" s="18" t="s">
         <v>36</v>
       </c>
@@ -5036,7 +5055,9 @@
         <v>8</v>
       </c>
       <c r="F53" s="17"/>
-      <c r="G53" s="17"/>
+      <c r="G53" s="17" t="s">
+        <v>169</v>
+      </c>
       <c r="H53" s="18" t="s">
         <v>79</v>
       </c>
@@ -10445,7 +10466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -11633,8 +11654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11741,7 +11762,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -11756,7 +11777,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -11774,11 +11795,11 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
@@ -11792,7 +11813,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -11810,7 +11831,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -11828,7 +11849,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -11846,7 +11867,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -11864,7 +11885,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -11912,32 +11933,48 @@
       <c r="A17" s="4">
         <v>1</v>
       </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="36" t="s">
-        <v>156</v>
-      </c>
-      <c r="E17" s="37"/>
+      <c r="B17" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D17" s="49"/>
+      <c r="E17" s="37" t="s">
+        <v>170</v>
+      </c>
       <c r="F17" s="38"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="4">
         <v>2</v>
       </c>
-      <c r="B18" s="35"/>
-      <c r="C18" s="4"/>
+      <c r="B18" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>162</v>
+      </c>
       <c r="D18" s="39"/>
-      <c r="E18" s="37"/>
+      <c r="E18" s="37" t="s">
+        <v>170</v>
+      </c>
       <c r="F18" s="38"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="4">
         <v>3</v>
       </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="4"/>
+      <c r="B19" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>162</v>
+      </c>
       <c r="D19" s="39"/>
-      <c r="E19" s="37"/>
+      <c r="E19" s="37" t="s">
+        <v>170</v>
+      </c>
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
i literally give up
</commit_message>
<xml_diff>
--- a/P13/Scrum.xlsx
+++ b/P13/Scrum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rachaelrocha/Documents/GitHub/cse1325/P13/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B963EF4-6E37-7A4E-AE1F-586739160CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D9A37A-C674-7445-A381-D20106C9515D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30160" windowHeight="17100" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="175">
   <si>
     <t>Product Name:</t>
   </si>
@@ -555,6 +555,18 @@
   </si>
   <si>
     <t>Completed Day 2</t>
+  </si>
+  <si>
+    <t>In Test</t>
+  </si>
+  <si>
+    <t>I CANT FIGURE IT OUT</t>
+  </si>
+  <si>
+    <t>In Work</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -2947,28 +2959,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-3</c:v>
+                  <c:v>-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-3</c:v>
+                  <c:v>-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3</c:v>
+                  <c:v>-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-3</c:v>
+                  <c:v>-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3</c:v>
+                  <c:v>-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-3</c:v>
+                  <c:v>-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3753,8 +3765,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I65" sqref="I65"/>
+    <sheetView topLeftCell="A49" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5084,7 +5096,9 @@
         <v>21</v>
       </c>
       <c r="F54" s="17"/>
-      <c r="G54" s="17"/>
+      <c r="G54" s="17" t="s">
+        <v>171</v>
+      </c>
       <c r="H54" s="18" t="s">
         <v>119</v>
       </c>
@@ -11655,7 +11669,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11762,7 +11776,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -11777,7 +11791,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -11795,7 +11809,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -11813,7 +11827,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -11831,7 +11845,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -11849,7 +11863,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -11867,7 +11881,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -11885,7 +11899,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -11920,7 +11934,7 @@
         <v>154</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="E16" s="33" t="s">
         <v>25</v>
@@ -11977,14 +11991,22 @@
       </c>
       <c r="F19" s="38"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="4">
         <v>4</v>
       </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="37"/>
+      <c r="B20" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D20" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="E20" s="37" t="s">
+        <v>173</v>
+      </c>
       <c r="F20" s="38"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">

</xml_diff>